<commit_message>
acessando yt com selenium
</commit_message>
<xml_diff>
--- a/g1/noticias.xlsx
+++ b/g1/noticias.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,136 +453,136 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Governo proíbe Meta de usar dados pessoais para treinar IA</t>
+          <t>Inflação argentina volta a subir após 5 meses e bate 271,5% em 1 ano</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Empresa de Mark Zuckerberg é responsável por WhatsApp, Instagram e Facebook.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2024/07/02/governo-manda-meta-suspender-politica-que-usa-dados-de-usuarios-para-treinar-inteligencia-artificial.ghtml</t>
+          <t>https://g1.globo.com/economia/noticia/2024/07/12/inflacao-argentina.ghtml</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Queda brusca arremessou passageiros para teto de avião; entenda</t>
+          <t>PF marca depoimento de Ramagem por espionagem no governo Bolsonaro</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/rn/rio-grande-do-norte/noticia/2024/07/02/especialistas-explicam-porque-passageiros-voaram-para-teto-de-aviao-durante-turbulencia-voo-desceu-cerca-de-150-metros.ghtml</t>
+          <t>https://g1.globo.com/politica/noticia/2024/07/12/pf-marca-para-quarta-feira-depoimento-de-ramagem-no-caso-da-abin-paralela.ghtml</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4 passageiros ainda estão na UTI em Natal após turbulência em voo</t>
+          <t>ANÁLISE: entrevista de Biden foi teste de cognição constrangedor</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Presidente dos EUA teve desempenho superior ao do debate, mas gafes roubaram a cena.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/rn/rio-grande-do-norte/noticia/2024/07/02/quatro-passageiros-de-voo-desviado-para-natal-apos-turbulencia-estao-na-uti.ghtml</t>
+          <t>https://g1.globo.com/mundo/blog/sandra-cohen/post/2024/07/12/biden-enfrenta-entrevista-como-um-constrangedor-teste-de-cognicao.ghtml</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Câmara de SP aprova Parque do Bixiga sem definir homenagem a Zé Celso</t>
+          <t>Governo avalia que 'Jogo do Tigrinho' pode ser liberado no Brasil</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Há vereadores que querem batizar local como Zé Celso, e outros, Silvio Santos.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/sp/sao-paulo/noticia/2024/07/02/camara-aprova-parques-do-bixiga-e-banespa-em-sao-paulo.ghtml</t>
+          <t>https://g1.globo.com/tecnologia/noticia/2024/07/12/governo-fortune-tiger-sites-exterior.ghtml</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Remédio para Alzheimer em estágios iniciais é aprovado nos EUA</t>
+          <t>Golpe do 'PIX errado': saiba como não ser enganado</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/saude/noticia/2024/07/02/droga-que-retarda-a-progressao-do-alzheimer-em-estagios-iniciais-fda.ghtml</t>
+          <t>https://g1.globo.com/economia/noticia/2024/07/12/golpe-do-pix-errado-saiba-como-os-criminosos-agem-e-como-nao-ser-enganado.ghtml</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Governo deve publicar regras para jogos de apostas, como o do 'tigrinho'</t>
+          <t>Polícia indicia 6 por morte de empresário com doce envenenado</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Namorada e mulher que se apresenta como cigana vão responder por homicídio.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/tecnologia/noticia/2024/07/02/portaria-que-regulamenta-jogos-on-line-deve-ser-publicada-neste-mes-diz-ministerio-da-fazenda.ghtml</t>
+          <t>https://g1.globo.com/rj/rio-de-janeiro/noticia/2024/07/12/policia-morte-de-empresario-envenenado-com-brigadeirao-no-rio.ghtml</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Xbox fica fora do ar para jogos com conexão em rede</t>
+          <t>GPS ajuda polícia dos EUA a prender suspeito de matar brasileira</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Corpo de Suzan Ferreira foi achado às margens de estrada em Michigan.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/pop-arte/games/noticia/2024/07/02/xbox-fora-do-ar-acesso-a-conta-e-perfil-enfrenta-problema-e-afeta-jogos-que-exigem-conexao.ghtml</t>
+          <t>https://g1.globo.com/mg/minas-gerais/noticia/2024/07/12/policia-americana-prende-suspeito-de-envolvimento-na-morte-de-brasileira-corpo-foi-encontrado-em-rodovia.ghtml</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lula defende cortar imposto só das carnes 'que o povo consome'</t>
+          <t>Nego Di é suspeito de lavagem de R$ 2 milhões com rifas; mulher é presa</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2024/07/02/lula-fala-em-reduzir-impostos-de-cortes-especificos-de-carne-na-cesta-basica-fiscalizacao-seria-impossivel-diz-secretario.ghtml</t>
+          <t>https://g1.globo.com/rs/rio-grande-do-sul/noticia/2024/07/12/nego-di-e-alvo-de-operacao-que-investiga-suspeita-de-lavagem-de-r-2-milhoes-com-rifas-virtuais.ghtml</t>
         </is>
       </c>
     </row>

</xml_diff>